<commit_message>
fixing the pfc footprints and relating them to their lcsc counterparts
</commit_message>
<xml_diff>
--- a/src/switched/pfc/LCSC_Exported_20210215_121240.xlsx
+++ b/src/switched/pfc/LCSC_Exported_20210215_121240.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
   <si>
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
@@ -449,6 +449,21 @@
   </si>
   <si>
     <t xml:space="preserve">lcsc.com/product-detail/Bridge-Rectifiers_MDD-Microdiode-Electronics-GBJ2510_C27523.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C601908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MO3W-82K±5%-QT73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">axial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82kΩ ±5% 3W ±350ppm/℃ Axial Metal Oxide Resistors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lcsc.com/product-detail/Metal-Oxide-Resistors_FlyWin-MO3W-82K-5-QT73_C601908.html</t>
   </si>
 </sst>
 </file>
@@ -531,13 +546,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -557,25 +584,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="135.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="153.24"/>
   </cols>
@@ -1462,6 +1489,41 @@
       </c>
       <c r="L25" s="0" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>0.0487</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Faster gate drive on pfc
</commit_message>
<xml_diff>
--- a/src/switched/pfc/LCSC_Exported_20210215_121240.xlsx
+++ b/src/switched/pfc/LCSC_Exported_20210215_121240.xlsx
@@ -196,19 +196,19 @@
     <t xml:space="preserve">lcsc.com/product-detail/Wirewound-Resistors_CCO-Chian-Chia-Elec-KNP2W-10Ω-5-T_C122131.html</t>
   </si>
   <si>
-    <t xml:space="preserve">C384297</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WR06X100JTL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walsin Tech Corp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10Ω ±5% 0.1W -200ppm/℃~+400ppm/℃ 0603 Chip Resistor - Surface Mount RoHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Walsin-Tech-Corp-WR06X100JTL_C384297.html</t>
+    <t xml:space="preserve">C217732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARG03FTC0130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viking Tech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 ±1% 1/10W 0603 High Precision &amp; Low TCR SMD Resistors RoHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://lcsc.com/product-detail/High-Precision-Low-TCR-SMD-Resistors_Viking-Tech-ARG03FTC0130_C217732.html</t>
   </si>
   <si>
     <t xml:space="preserve">C393080</t>
@@ -589,7 +589,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -960,14 +960,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -980,16 +980,16 @@
         <v>16</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>0.0012</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>0.12</v>
+        <v>50</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0.0119</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>0.6</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
Low effort input filter added to pfc, vestigial input port remains for potential issues
</commit_message>
<xml_diff>
--- a/src/switched/pfc/LCSC_Exported_20210215_121240.xlsx
+++ b/src/switched/pfc/LCSC_Exported_20210215_121240.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="159">
   <si>
     <t xml:space="preserve">LCSC Part Number</t>
   </si>
@@ -464,6 +464,39 @@
   </si>
   <si>
     <t xml:space="preserve">lcsc.com/product-detail/Bridge-Rectifiers_DIYI-Elec-Tech-ABS10_C84158.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C710468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NM1206B104K451CEGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUI JU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100nF ±10% 450V X7R 1206 Multilayer Ceramic Capacitors MLCC - SMD/SMT RoHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_HUI-JU-NM1206B104K451CEGN_C710468.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C357261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMPC1206HP-220MG-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAI-TECH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD,13.5x12.5x5.7mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22uH ±20% 8A 34mΩ SMD,13.5x12.5x5.7mm Power Inductors RoHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lcsc.com/product-detail/Power-Inductors_TAI-TECH-TMPC1206HP-220MG-D_C357261.html</t>
   </si>
 </sst>
 </file>
@@ -584,12 +617,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="36:37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1526,6 +1559,76 @@
         <v>147</v>
       </c>
     </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>1206</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>0.0233</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>0.6312</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>